<commit_message>
v1.3 Implementacion de BD para calcular la nota
correciones de errores y arreglos a algunas funciones
</commit_message>
<xml_diff>
--- a/Material de Apoyo/Rubrica.xlsx
+++ b/Material de Apoyo/Rubrica.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Notas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Notas\Material de Apoyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23ADFC4-DDB0-4E69-B9B8-AA18C078EE1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0771E5CF-D5D1-4139-B869-D566E5BAED38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="1605" windowWidth="16620" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6435" yWindow="1995" windowWidth="16620" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>intro</t>
   </si>
@@ -50,6 +51,12 @@
   </si>
   <si>
     <t>Total 2</t>
+  </si>
+  <si>
+    <t>puntaje</t>
+  </si>
+  <si>
+    <t>nota</t>
   </si>
 </sst>
 </file>
@@ -446,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J137"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,7 +1828,7 @@
   <dimension ref="A1:I137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,16 +1870,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>0.1</v>
@@ -1887,16 +1894,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>0.2</v>
@@ -1911,10 +1918,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1945,19 +1952,19 @@
       </c>
       <c r="C7">
         <f t="shared" ref="C7:F7" si="1">SUM(C3:C5)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <v>0.5</v>
@@ -2022,19 +2029,19 @@
       </c>
       <c r="C11">
         <f t="shared" ref="C11:F11" si="2">C7*C9</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H11">
         <v>0.9</v>
@@ -2056,7 +2063,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <f>SUM(B11:F11)*0.01</f>
-        <v>0.6</v>
+        <v>2.7</v>
       </c>
       <c r="H13">
         <v>1.1000000000000001</v>
@@ -2069,7 +2076,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f>ROUND(TRUNC(IF(B13&lt;8.1,3*B13/8.1+1,3*(B13-8.1)/5.4+4),2),1)</f>
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="H14">
         <v>1.2</v>
@@ -2103,20 +2110,20 @@
         <v>0.6</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:F17" si="3">C11*0.01</f>
-        <v>0</v>
+        <f t="shared" ref="C17:E17" si="3">C11*0.01</f>
+        <v>0.9</v>
       </c>
       <c r="D17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>F11*0.01</f>
+        <v>0.4</v>
       </c>
       <c r="H17">
         <v>1.5</v>
@@ -3217,4 +3224,1251 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2F7340-5FCF-4B0C-96C1-C36F5FB0A9E1}">
+  <dimension ref="A1:B137"/>
+  <sheetViews>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="E127" sqref="E127"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B65" si="0">ROUND(TRUNC(IF(A2&lt;8.1,3*A2/8.1+1,3*(A2-8.1)/5.4+4),2),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.1</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.2</v>
+      </c>
+      <c r="B4" s="1">
+        <f>ROUND(TRUNC(IF(A4&lt;8.1,3*A4/8.1+1,3*(A4-8.1)/5.4+4),2),1)</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.3</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.4</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.5</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.6</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.7</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.8</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.9</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1.2</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1.3</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1.4</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1.5</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1.6</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1.7</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1.8</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1.9</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2.1</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2.4</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2.5</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2.6</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2.7</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2.8</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2.9</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3.1</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3.2</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3.3</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>3.4</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3.5</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3.6</v>
+      </c>
+      <c r="B38" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3.7</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3.8</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>3.9</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B43" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>4.2</v>
+      </c>
+      <c r="B44" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>4.3</v>
+      </c>
+      <c r="B45" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B46" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>4.5</v>
+      </c>
+      <c r="B47" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>4.7</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>4.8</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>5</v>
+      </c>
+      <c r="B52" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B53" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>5.2</v>
+      </c>
+      <c r="B54" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>5.3</v>
+      </c>
+      <c r="B55" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>5.4</v>
+      </c>
+      <c r="B56" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>5.5</v>
+      </c>
+      <c r="B57" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>5.6</v>
+      </c>
+      <c r="B58" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>5.7</v>
+      </c>
+      <c r="B59" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>5.8</v>
+      </c>
+      <c r="B60" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>5.9</v>
+      </c>
+      <c r="B61" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>6</v>
+      </c>
+      <c r="B62" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>6.1</v>
+      </c>
+      <c r="B63" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>6.2</v>
+      </c>
+      <c r="B64" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>6.3</v>
+      </c>
+      <c r="B65" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>6.4</v>
+      </c>
+      <c r="B66" s="1">
+        <f t="shared" ref="B66:B129" si="1">ROUND(TRUNC(IF(A66&lt;8.1,3*A66/8.1+1,3*(A66-8.1)/5.4+4),2),1)</f>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>6.5</v>
+      </c>
+      <c r="B67" s="1">
+        <f t="shared" si="1"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>6.6</v>
+      </c>
+      <c r="B68" s="1">
+        <f t="shared" si="1"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>6.7</v>
+      </c>
+      <c r="B69" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>6.8</v>
+      </c>
+      <c r="B70" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>6.9</v>
+      </c>
+      <c r="B71" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>7</v>
+      </c>
+      <c r="B72" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>7.1</v>
+      </c>
+      <c r="B73" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>7.2</v>
+      </c>
+      <c r="B74" s="1">
+        <f t="shared" si="1"/>
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>7.3</v>
+      </c>
+      <c r="B75" s="1">
+        <f t="shared" si="1"/>
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>7.4</v>
+      </c>
+      <c r="B76" s="1">
+        <f t="shared" si="1"/>
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>7.5</v>
+      </c>
+      <c r="B77" s="1">
+        <f t="shared" si="1"/>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>7.6</v>
+      </c>
+      <c r="B78" s="1">
+        <f t="shared" si="1"/>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>7.7</v>
+      </c>
+      <c r="B79" s="1">
+        <f t="shared" si="1"/>
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>7.8</v>
+      </c>
+      <c r="B80" s="1">
+        <f t="shared" si="1"/>
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>7.9</v>
+      </c>
+      <c r="B81" s="1">
+        <f t="shared" si="1"/>
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>8</v>
+      </c>
+      <c r="B82" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>8.1</v>
+      </c>
+      <c r="B83" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B84" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B85" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>8.4</v>
+      </c>
+      <c r="B86" s="1">
+        <f t="shared" si="1"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>8.5</v>
+      </c>
+      <c r="B87" s="1">
+        <f t="shared" si="1"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>8.6</v>
+      </c>
+      <c r="B88" s="1">
+        <f t="shared" si="1"/>
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="B89" s="1">
+        <f t="shared" si="1"/>
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="B90" s="1">
+        <f t="shared" si="1"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>8.9</v>
+      </c>
+      <c r="B91" s="1">
+        <f t="shared" si="1"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>9</v>
+      </c>
+      <c r="B92" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>9.1</v>
+      </c>
+      <c r="B93" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B94" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="B95" s="1">
+        <f t="shared" si="1"/>
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>9.4</v>
+      </c>
+      <c r="B96" s="1">
+        <f t="shared" si="1"/>
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>9.5</v>
+      </c>
+      <c r="B97" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>9.6</v>
+      </c>
+      <c r="B98" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="B99" s="1">
+        <f t="shared" si="1"/>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="B100" s="1">
+        <f t="shared" si="1"/>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>9.9</v>
+      </c>
+      <c r="B101" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>10</v>
+      </c>
+      <c r="B102" s="1">
+        <f t="shared" si="1"/>
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>10.1</v>
+      </c>
+      <c r="B103" s="1">
+        <f t="shared" si="1"/>
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B104" s="1">
+        <f t="shared" si="1"/>
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>10.3</v>
+      </c>
+      <c r="B105" s="1">
+        <f t="shared" si="1"/>
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>10.4</v>
+      </c>
+      <c r="B106" s="1">
+        <f t="shared" si="1"/>
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>10.5</v>
+      </c>
+      <c r="B107" s="1">
+        <f t="shared" si="1"/>
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>10.6</v>
+      </c>
+      <c r="B108" s="1">
+        <f t="shared" si="1"/>
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>10.7</v>
+      </c>
+      <c r="B109" s="1">
+        <f t="shared" si="1"/>
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>10.8</v>
+      </c>
+      <c r="B110" s="1">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>10.9</v>
+      </c>
+      <c r="B111" s="1">
+        <f t="shared" si="1"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>11</v>
+      </c>
+      <c r="B112" s="1">
+        <f t="shared" si="1"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>11.1</v>
+      </c>
+      <c r="B113" s="1">
+        <f t="shared" si="1"/>
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>11.2</v>
+      </c>
+      <c r="B114" s="1">
+        <f t="shared" si="1"/>
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>11.3</v>
+      </c>
+      <c r="B115" s="1">
+        <f t="shared" si="1"/>
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>11.4</v>
+      </c>
+      <c r="B116" s="1">
+        <f t="shared" si="1"/>
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>11.5</v>
+      </c>
+      <c r="B117" s="1">
+        <f t="shared" si="1"/>
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>11.6</v>
+      </c>
+      <c r="B118" s="1">
+        <f t="shared" si="1"/>
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>11.7</v>
+      </c>
+      <c r="B119" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>11.8</v>
+      </c>
+      <c r="B120" s="1">
+        <f t="shared" si="1"/>
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>11.9</v>
+      </c>
+      <c r="B121" s="1">
+        <f t="shared" si="1"/>
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>12</v>
+      </c>
+      <c r="B122" s="1">
+        <f t="shared" si="1"/>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>12.1</v>
+      </c>
+      <c r="B123" s="1">
+        <f t="shared" si="1"/>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>12.2</v>
+      </c>
+      <c r="B124" s="1">
+        <f t="shared" si="1"/>
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>12.3</v>
+      </c>
+      <c r="B125" s="1">
+        <f t="shared" si="1"/>
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>12.4</v>
+      </c>
+      <c r="B126" s="1">
+        <f t="shared" si="1"/>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>12.5</v>
+      </c>
+      <c r="B127" s="1">
+        <f t="shared" si="1"/>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>12.6</v>
+      </c>
+      <c r="B128" s="1">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>12.7</v>
+      </c>
+      <c r="B129" s="1">
+        <f t="shared" si="1"/>
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>12.8</v>
+      </c>
+      <c r="B130" s="1">
+        <f t="shared" ref="B130:B137" si="2">ROUND(TRUNC(IF(A130&lt;8.1,3*A130/8.1+1,3*(A130-8.1)/5.4+4),2),1)</f>
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>12.9</v>
+      </c>
+      <c r="B131" s="1">
+        <f t="shared" si="2"/>
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>13</v>
+      </c>
+      <c r="B132" s="1">
+        <f t="shared" si="2"/>
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>13.1</v>
+      </c>
+      <c r="B133" s="1">
+        <f t="shared" si="2"/>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>13.2</v>
+      </c>
+      <c r="B134" s="1">
+        <f t="shared" si="2"/>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>13.3</v>
+      </c>
+      <c r="B135" s="1">
+        <f t="shared" si="2"/>
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>13.4</v>
+      </c>
+      <c r="B136" s="1">
+        <f t="shared" si="2"/>
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>13.5</v>
+      </c>
+      <c r="B137" s="1">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>